<commit_message>
english of some questions added
</commit_message>
<xml_diff>
--- a/DB and Documents/WASHB_DRAFT_MLHEFather.xlsx
+++ b/DB and Documents/WASHB_DRAFT_MLHEFather.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="269">
   <si>
     <t>SLNo</t>
   </si>
@@ -686,9 +686,6 @@
   </si>
   <si>
     <t>202.KZ Nb Nb Avcwb Avcbvi cwiev‡ii m`m¨‡`i ˆ`bw›`b Rxe‡bi wbivcËv wb‡q wPwšÍZ - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?</t>
-  </si>
-  <si>
-    <t>203.KZ Nb Nb Avcwb Avcbvi cwiev‡ii m`m¨‡`i ˆ`bw›`b Rxe‡bi wbivcËv wb‡q wPwšÍZ - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?</t>
   </si>
   <si>
     <t>204.KZ Nb Nb Avcbvi g‡b nq †h Avcbvi Kv‡Q cwiev‡ii LiP Pvjv‡bvi gZ ch©vß UvKv Av‡Q ev DcvR©b K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?</t>
@@ -839,6 +836,51 @@
   </si>
   <si>
     <t>4.Very Often</t>
+  </si>
+  <si>
+    <t>201.How often do you worry about your safety in your daily life – Never, Almost Never, Sometimes, Fairly Often, Very Often?</t>
+  </si>
+  <si>
+    <t>202.How often do you worry about your family’s safety in their daily lives – Never, Almost Never, Sometimes, Fairly Often, Very Often?</t>
+  </si>
+  <si>
+    <t>203.How often do you feel that you have/make enough money to support yourself – Never, Almost Never, Sometimes, Fairly Often, Very Often?</t>
+  </si>
+  <si>
+    <t>203.KZ Nb Nb Avcbvi g‡b nq †h Avcbvi Kv‡Q wb‡Ri LiP Pjvi gZ ch©vß UvKv Av‡Q ev DcvR©b K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?</t>
+  </si>
+  <si>
+    <t>204.How often do you feel that you have/make enough money to support your family – Never, Almost Never, Sometimes, Fairly Often, Very Often?</t>
+  </si>
+  <si>
+    <t>205.How often do you worry about being able to feed yourself and your family – Never, Almost Never, Sometimes, Fairly Often, Very Often?</t>
+  </si>
+  <si>
+    <t>206.How often do you worry about having a house for you and your family to sleep in – Never, Almost Never, Sometimes, Fairly Often, Very Often?</t>
+  </si>
+  <si>
+    <t>207.How often do you get to make decisions at your work (as opposed to follow directions) – Never, Almost Never, Sometimes, Fairly Often, Very Often?</t>
+  </si>
+  <si>
+    <t>208.How often do you like your boss – Never, Almost Never, Sometimes, Fairly Often, Very Often?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">209.How often do you enjoy your job – Never, Almost Never, Sometimes, Fairly Often, Very Often?  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">210.During your week how often do you get to do something fun for yourself – Never, Almost Never, Sometimes, Fairly Often, Very Often?  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">212.How often do you worry about your health – Never, Almost Never, Sometimes, Fairly Often, Very Often? </t>
+  </si>
+  <si>
+    <t>212.How often do you worry about your family’s health – Never, Almost Never, Sometimes, Fairly Often, Very Often?</t>
+  </si>
+  <si>
+    <t>213.How often do you have people in your life who will support you if you need it? For example, if you are feeling sad? If you need someone to look after your child – Never, Almost Never, Sometimes, Fairly Often, Very Often?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">214.How often do you take care of your parents or your wife’s parents – Never, Almost Never, Sometimes, Fairly Often, Very Often?  </t>
   </si>
 </sst>
 </file>
@@ -2656,8 +2698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O61" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V71"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2806,7 +2848,7 @@
         <v>40</v>
       </c>
       <c r="V3" t="str">
-        <f t="shared" ref="V3:V37" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
+        <f t="shared" ref="V3:V11" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('2', 'q1','frmcombobox', 'tblMainQues','1.mv¶vrKviMÖnYKvixiAvBwW','1.ID of MT/FRA/FRO','','q2','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
@@ -4097,7 +4139,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('37', 'msg202','frmmessage', 'tblMainQues','Avcbv‡K Avcbvi Abyf~wZ Ges wPšÍv-fvebv m¤ú‡K© wKQy cÖkœ Kie| cÖ‡Z¨K †¶‡ÎB, Avcwb KZ Nb Nb Abyfe K‡ib ev wPšÍv K‡ib Zv ej‡Z n‡e|','The questions in this scale ask you about your feelings and thoughts . In each case, you will be asked to indicate how often you felt or thought a certain way.','','q201','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="78.75">
+    <row r="39" spans="1:22" ht="90">
       <c r="A39" s="90">
         <v>38</v>
       </c>
@@ -4112,6 +4154,9 @@
       </c>
       <c r="E39" s="71" t="s">
         <v>209</v>
+      </c>
+      <c r="F39" s="91" t="s">
+        <v>254</v>
       </c>
       <c r="H39" s="90" t="s">
         <v>181</v>
@@ -4128,10 +4173,10 @@
       <c r="U39" s="161"/>
       <c r="V39" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('38', 'q201','frmsinglechoice', 'tblMainQues','201.KZ Nb Nb Avcwb Avcbvi ˆ`bw›`b Rxe‡bi wbivcËv wb‡q wPwšÍZ - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q202','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" ht="94.5">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('38', 'q201','frmsinglechoice', 'tblMainQues','201.KZ Nb Nb Avcwb Avcbvi ˆ`bw›`b Rxe‡bi wbivcËv wb‡q wPwšÍZ - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','201.How often do you worry about your safety in your daily life – Never, Almost Never, Sometimes, Fairly Often, Very Often?','','q202','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="105">
       <c r="A40" s="90">
         <v>39</v>
       </c>
@@ -4146,6 +4191,9 @@
       </c>
       <c r="E40" s="71" t="s">
         <v>210</v>
+      </c>
+      <c r="F40" s="91" t="s">
+        <v>255</v>
       </c>
       <c r="H40" s="90" t="s">
         <v>182</v>
@@ -4162,10 +4210,10 @@
       <c r="U40" s="161"/>
       <c r="V40" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('39', 'q202','frmsinglechoice', 'tblMainQues','202.KZ Nb Nb Avcwb Avcbvi cwiev‡ii m`m¨‡`i ˆ`bw›`b Rxe‡bi wbivcËv wb‡q wPwšÍZ - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q203','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" ht="94.5">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('39', 'q202','frmsinglechoice', 'tblMainQues','202.KZ Nb Nb Avcwb Avcbvi cwiev‡ii m`m¨‡`i ˆ`bw›`b Rxe‡bi wbivcËv wb‡q wPwšÍZ - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','202.How often do you worry about your family’s safety in their daily lives – Never, Almost Never, Sometimes, Fairly Often, Very Often?','','q203','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" ht="120">
       <c r="A41" s="90">
         <v>40</v>
       </c>
@@ -4178,8 +4226,11 @@
       <c r="D41" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="71" t="s">
-        <v>211</v>
+      <c r="E41" s="85" t="s">
+        <v>257</v>
+      </c>
+      <c r="F41" s="91" t="s">
+        <v>256</v>
       </c>
       <c r="H41" s="90" t="s">
         <v>183</v>
@@ -4196,10 +4247,10 @@
       <c r="U41" s="161"/>
       <c r="V41" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('40', 'q203','frmsinglechoice', 'tblMainQues','203.KZ Nb Nb Avcwb Avcbvi cwiev‡ii m`m¨‡`i ˆ`bw›`b Rxe‡bi wbivcËv wb‡q wPwšÍZ - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q204','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" ht="110.25">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('40', 'q203','frmsinglechoice', 'tblMainQues','203.KZ Nb Nb Avcbvi g‡b nq †h Avcbvi Kv‡Q wb‡Ri LiP Pjvi gZ ch©vß UvKv Av‡Q ev DcvR©b K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','203.How often do you feel that you have/make enough money to support yourself – Never, Almost Never, Sometimes, Fairly Often, Very Often?','','q204','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" ht="120">
       <c r="A42" s="90">
         <v>41</v>
       </c>
@@ -4213,7 +4264,10 @@
         <v>42</v>
       </c>
       <c r="E42" s="71" t="s">
-        <v>212</v>
+        <v>211</v>
+      </c>
+      <c r="F42" s="91" t="s">
+        <v>258</v>
       </c>
       <c r="H42" s="90" t="s">
         <v>184</v>
@@ -4230,7 +4284,7 @@
       <c r="U42" s="161"/>
       <c r="V42" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('41', 'q204','frmsinglechoice', 'tblMainQues','204.KZ Nb Nb Avcbvi g‡b nq †h Avcbvi Kv‡Q cwiev‡ii LiP Pvjv‡bvi gZ ch©vß UvKv Av‡Q ev DcvR©b K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q205','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('41', 'q204','frmsinglechoice', 'tblMainQues','204.KZ Nb Nb Avcbvi g‡b nq †h Avcbvi Kv‡Q cwiev‡ii LiP Pvjv‡bvi gZ ch©vß UvKv Av‡Q ev DcvR©b K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','204.How often do you feel that you have/make enough money to support your family – Never, Almost Never, Sometimes, Fairly Often, Very Often?','','q205','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="110.25">
@@ -4247,7 +4301,10 @@
         <v>42</v>
       </c>
       <c r="E43" s="71" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="F43" s="91" t="s">
+        <v>259</v>
       </c>
       <c r="H43" s="90" t="s">
         <v>185</v>
@@ -4264,7 +4321,7 @@
       <c r="U43" s="161"/>
       <c r="V43" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('42', 'q205','frmsinglechoice', 'tblMainQues','205.Avcwb KZ Nb Nb Avcbvi Ges Avcbvi cwiev‡ii m`m¨‡`i LvIqv‡Z cvi‡eb wKbv Zv wb‡q `ywðšÍv K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q206','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('42', 'q205','frmsinglechoice', 'tblMainQues','205.Avcwb KZ Nb Nb Avcbvi Ges Avcbvi cwiev‡ii m`m¨‡`i LvIqv‡Z cvi‡eb wKbv Zv wb‡q `ywðšÍv K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','205.How often do you worry about being able to feed yourself and your family – Never, Almost Never, Sometimes, Fairly Often, Very Often?','','q206','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="110.25">
@@ -4281,7 +4338,10 @@
         <v>42</v>
       </c>
       <c r="E44" s="71" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="F44" s="91" t="s">
+        <v>260</v>
       </c>
       <c r="H44" s="90" t="s">
         <v>186</v>
@@ -4298,10 +4358,10 @@
       <c r="U44" s="161"/>
       <c r="V44" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('43', 'q206','frmsinglechoice', 'tblMainQues','206.Avcwb KZ Nb Nb Avcbvi Ges Avcbvi cwiev‡ii m`m¨‡`i Rb¨ GKwU evwo _vK‡e wKbv Zv wb‡q  `ywðšÍv K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB? ','','','q207','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" ht="94.5">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('43', 'q206','frmsinglechoice', 'tblMainQues','206.Avcwb KZ Nb Nb Avcbvi Ges Avcbvi cwiev‡ii m`m¨‡`i Rb¨ GKwU evwo _vK‡e wKbv Zv wb‡q  `ywðšÍv K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB? ','206.How often do you worry about having a house for you and your family to sleep in – Never, Almost Never, Sometimes, Fairly Often, Very Often?','','q207','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" ht="120">
       <c r="A45" s="90">
         <v>44</v>
       </c>
@@ -4315,7 +4375,10 @@
         <v>42</v>
       </c>
       <c r="E45" s="71" t="s">
-        <v>215</v>
+        <v>214</v>
+      </c>
+      <c r="F45" s="91" t="s">
+        <v>261</v>
       </c>
       <c r="H45" s="90" t="s">
         <v>187</v>
@@ -4332,7 +4395,7 @@
       <c r="U45" s="161"/>
       <c r="V45" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('44', 'q207','frmsinglechoice', 'tblMainQues','207.KZ Nb Nb Avcwb Avcbvi Kg©‡¶‡Î wm×všÍ MÖnY Ki‡Z cv‡ib (wb‡`©kbv Abymi‡Yi wecix‡Z) - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q208','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('44', 'q207','frmsinglechoice', 'tblMainQues','207.KZ Nb Nb Avcwb Avcbvi Kg©‡¶‡Î wm×všÍ MÖnY Ki‡Z cv‡ib (wb‡`©kbv Abymi‡Yi wecix‡Z) - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','207.How often do you get to make decisions at your work (as opposed to follow directions) – Never, Almost Never, Sometimes, Fairly Often, Very Often?','','q208','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="78.75">
@@ -4349,7 +4412,10 @@
         <v>42</v>
       </c>
       <c r="E46" s="71" t="s">
-        <v>216</v>
+        <v>215</v>
+      </c>
+      <c r="F46" s="91" t="s">
+        <v>262</v>
       </c>
       <c r="H46" s="90" t="s">
         <v>188</v>
@@ -4366,7 +4432,7 @@
       <c r="U46" s="161"/>
       <c r="V46" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('45', 'q208','frmsinglechoice', 'tblMainQues','208.KZ Nb Nb Avcbvi g‡b nq Avcwb Avcbvi em/m¨vi ‡K cQ›` K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q209','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('45', 'q208','frmsinglechoice', 'tblMainQues','208.KZ Nb Nb Avcbvi g‡b nq Avcwb Avcbvi em/m¨vi ‡K cQ›` K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','208.How often do you like your boss – Never, Almost Never, Sometimes, Fairly Often, Very Often?','','q209','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="94.5">
@@ -4383,7 +4449,10 @@
         <v>42</v>
       </c>
       <c r="E47" s="71" t="s">
-        <v>217</v>
+        <v>216</v>
+      </c>
+      <c r="F47" s="91" t="s">
+        <v>263</v>
       </c>
       <c r="H47" s="90" t="s">
         <v>189</v>
@@ -4400,10 +4469,10 @@
       <c r="U47" s="161"/>
       <c r="V47" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('46', 'q209','frmsinglechoice', 'tblMainQues','209.KZ Nb Nb Avcwb Avcbvi PvKzix/Kg©‡¶Î/KvR‡K Dc‡fvM K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q210','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22" ht="78.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('46', 'q209','frmsinglechoice', 'tblMainQues','209.KZ Nb Nb Avcwb Avcbvi PvKzix/Kg©‡¶Î/KvR‡K Dc‡fvM K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','209.How often do you enjoy your job – Never, Almost Never, Sometimes, Fairly Often, Very Often?  ','','q210','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" ht="105">
       <c r="A48" s="90">
         <v>47</v>
       </c>
@@ -4417,7 +4486,10 @@
         <v>42</v>
       </c>
       <c r="E48" s="71" t="s">
-        <v>218</v>
+        <v>217</v>
+      </c>
+      <c r="F48" s="91" t="s">
+        <v>264</v>
       </c>
       <c r="H48" s="90" t="s">
         <v>190</v>
@@ -4434,10 +4506,10 @@
       <c r="U48" s="161"/>
       <c r="V48" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('47', 'q210','frmsinglechoice', 'tblMainQues','210.KZ Nb Nb Avcwb Avcbvi wb‡Ri Avb‡›`i Rb¨ wKQy Ki‡Z cv‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q211','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22" ht="78.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('47', 'q210','frmsinglechoice', 'tblMainQues','210.KZ Nb Nb Avcwb Avcbvi wb‡Ri Avb‡›`i Rb¨ wKQy Ki‡Z cv‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','210.During your week how often do you get to do something fun for yourself – Never, Almost Never, Sometimes, Fairly Often, Very Often?  ','','q211','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="90">
       <c r="A49" s="90">
         <v>48</v>
       </c>
@@ -4450,8 +4522,11 @@
       <c r="D49" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="E49" s="71" t="s">
-        <v>219</v>
+      <c r="E49" s="85" t="s">
+        <v>218</v>
+      </c>
+      <c r="F49" s="91" t="s">
+        <v>265</v>
       </c>
       <c r="H49" s="90" t="s">
         <v>191</v>
@@ -4468,10 +4543,10 @@
       <c r="U49" s="161"/>
       <c r="V49" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('48', 'q211','frmsinglechoice', 'tblMainQues','211.KZ Nb Nb Avcwb Avcbvi ¯^v¯’¨ wb‡q wPšvÍ K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q212','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
-      </c>
-    </row>
-    <row r="50" spans="1:22" ht="78.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('48', 'q211','frmsinglechoice', 'tblMainQues','211.KZ Nb Nb Avcwb Avcbvi ¯^v¯’¨ wb‡q wPšvÍ K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','212.How often do you worry about your health – Never, Almost Never, Sometimes, Fairly Often, Very Often? ','','q212','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" ht="90">
       <c r="A50" s="90">
         <v>49</v>
       </c>
@@ -4485,7 +4560,10 @@
         <v>42</v>
       </c>
       <c r="E50" s="71" t="s">
-        <v>220</v>
+        <v>219</v>
+      </c>
+      <c r="F50" s="91" t="s">
+        <v>266</v>
       </c>
       <c r="H50" s="90" t="s">
         <v>192</v>
@@ -4502,10 +4580,10 @@
       <c r="U50" s="161"/>
       <c r="V50" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('49', 'q212','frmsinglechoice', 'tblMainQues','212.KZ Nb Nb Avcwb Avcbvi cwiev‡ii m`m¨‡`i ¯^v¯’¨ wb‡q wPšvÍ K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q213','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" ht="141.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('49', 'q212','frmsinglechoice', 'tblMainQues','212.KZ Nb Nb Avcwb Avcbvi cwiev‡ii m`m¨‡`i ¯^v¯’¨ wb‡q wPšvÍ K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','212.How often do you worry about your family’s health – Never, Almost Never, Sometimes, Fairly Often, Very Often?','','q213','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="165">
       <c r="A51" s="90">
         <v>50</v>
       </c>
@@ -4519,7 +4597,10 @@
         <v>42</v>
       </c>
       <c r="E51" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
+      </c>
+      <c r="F51" s="91" t="s">
+        <v>267</v>
       </c>
       <c r="H51" s="90" t="s">
         <v>193</v>
@@ -4536,10 +4617,10 @@
       <c r="U51" s="161"/>
       <c r="V51" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('50', 'q213','frmsinglechoice', 'tblMainQues','213.KZ Nb Nb Avcbvi g‡b nq, Avcbvi Rxe‡b Ggb †Kvb gvbyl Av‡Q †h Avcbvi cÖ‡qvR‡b Avcbv‡K mvnvh¨ Ki‡e (†hgb gb Lvivc n‡j ev wkï‡K †`Lvïbv Kivi cÖ‡qvRb n‡j) - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','q214','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22" ht="95.25" thickBot="1">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('50', 'q213','frmsinglechoice', 'tblMainQues','213.KZ Nb Nb Avcbvi g‡b nq, Avcbvi Rxe‡b Ggb †Kvb gvbyl Av‡Q †h Avcbvi cÖ‡qvR‡b Avcbv‡K mvnvh¨ Ki‡e (†hgb gb Lvivc n‡j ev wkï‡K †`Lvïbv Kivi cÖ‡qvRb n‡j) - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','213.How often do you have people in your life who will support you if you need it? For example, if you are feeling sad? If you need someone to look after your child – Never, Almost Never, Sometimes, Fairly Often, Very Often?','','q214','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="105.75" thickBot="1">
       <c r="A52" s="90">
         <v>51</v>
       </c>
@@ -4553,7 +4634,10 @@
         <v>42</v>
       </c>
       <c r="E52" s="71" t="s">
-        <v>222</v>
+        <v>221</v>
+      </c>
+      <c r="F52" s="91" t="s">
+        <v>268</v>
       </c>
       <c r="H52" s="90" t="s">
         <v>204</v>
@@ -4570,7 +4654,7 @@
       <c r="U52" s="161"/>
       <c r="V52" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('51', 'q214','frmsinglechoice', 'tblMainQues','214.KZ Nb Nb Avcwb Avcbvi evev-gv ev Avcbvi ¯¿xi evev-gv †K †`Lvïbv K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','','','msg203','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('51', 'q214','frmsinglechoice', 'tblMainQues','214.KZ Nb Nb Avcwb Avcbvi evev-gv ev Avcbvi ¯¿xi evev-gv †K †`Lvïbv K‡ib - KLbB bv, K`vwPr, gv‡S g‡a¨, Nb Nb bvwK cÖvqB?','214.How often do you take care of your parents or your wife’s parents – Never, Almost Never, Sometimes, Fairly Often, Very Often?  ','','msg203','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="53" spans="1:22" ht="175.5">
@@ -4587,10 +4671,10 @@
         <v>42</v>
       </c>
       <c r="E53" s="78" t="s">
+        <v>222</v>
+      </c>
+      <c r="F53" s="79" t="s">
         <v>223</v>
-      </c>
-      <c r="F53" s="79" t="s">
-        <v>224</v>
       </c>
       <c r="H53" s="90" t="s">
         <v>194</v>
@@ -4624,10 +4708,10 @@
         <v>42</v>
       </c>
       <c r="E54" s="81" t="s">
+        <v>224</v>
+      </c>
+      <c r="F54" s="80" t="s">
         <v>225</v>
-      </c>
-      <c r="F54" s="80" t="s">
-        <v>226</v>
       </c>
       <c r="H54" s="90" t="s">
         <v>195</v>
@@ -4661,10 +4745,10 @@
         <v>42</v>
       </c>
       <c r="E55" s="81" t="s">
+        <v>226</v>
+      </c>
+      <c r="F55" s="80" t="s">
         <v>227</v>
-      </c>
-      <c r="F55" s="80" t="s">
-        <v>228</v>
       </c>
       <c r="H55" s="90" t="s">
         <v>196</v>
@@ -4698,10 +4782,10 @@
         <v>42</v>
       </c>
       <c r="E56" s="81" t="s">
+        <v>228</v>
+      </c>
+      <c r="F56" s="80" t="s">
         <v>229</v>
-      </c>
-      <c r="F56" s="80" t="s">
-        <v>230</v>
       </c>
       <c r="H56" s="90" t="s">
         <v>197</v>
@@ -4735,10 +4819,10 @@
         <v>42</v>
       </c>
       <c r="E57" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="F57" s="82" t="s">
         <v>231</v>
-      </c>
-      <c r="F57" s="82" t="s">
-        <v>232</v>
       </c>
       <c r="H57" s="90" t="s">
         <v>198</v>
@@ -4772,10 +4856,10 @@
         <v>42</v>
       </c>
       <c r="E58" s="85" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F58" s="84" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H58" s="90" t="s">
         <v>199</v>
@@ -4809,10 +4893,10 @@
         <v>42</v>
       </c>
       <c r="E59" s="85" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F59" s="86" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H59" s="90" t="s">
         <v>200</v>
@@ -4846,10 +4930,10 @@
         <v>42</v>
       </c>
       <c r="E60" s="85" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F60" s="87" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H60" s="90" t="s">
         <v>201</v>
@@ -4883,10 +4967,10 @@
         <v>42</v>
       </c>
       <c r="E61" s="85" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F61" s="88" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H61" s="90" t="s">
         <v>202</v>
@@ -4920,10 +5004,10 @@
         <v>42</v>
       </c>
       <c r="E62" s="85" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F62" s="89" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H62" s="90" t="s">
         <v>203</v>
@@ -4957,10 +5041,10 @@
         <v>42</v>
       </c>
       <c r="E63" s="85" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F63" s="91" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H63" s="90" t="s">
         <v>146</v>
@@ -6270,10 +6354,10 @@
         <v>180</v>
       </c>
       <c r="C43" s="93" t="s">
+        <v>244</v>
+      </c>
+      <c r="D43" s="92" t="s">
         <v>245</v>
-      </c>
-      <c r="D43" s="92" t="s">
-        <v>246</v>
       </c>
       <c r="E43" s="94">
         <v>0</v>
@@ -6289,10 +6373,10 @@
         <v>180</v>
       </c>
       <c r="C44" s="93" t="s">
+        <v>246</v>
+      </c>
+      <c r="D44" s="92" t="s">
         <v>247</v>
-      </c>
-      <c r="D44" s="92" t="s">
-        <v>248</v>
       </c>
       <c r="E44" s="94">
         <v>1</v>
@@ -6309,10 +6393,10 @@
         <v>180</v>
       </c>
       <c r="C45" s="93" t="s">
+        <v>248</v>
+      </c>
+      <c r="D45" s="92" t="s">
         <v>249</v>
-      </c>
-      <c r="D45" s="92" t="s">
-        <v>250</v>
       </c>
       <c r="E45" s="94">
         <v>2</v>
@@ -6329,10 +6413,10 @@
         <v>180</v>
       </c>
       <c r="C46" s="93" t="s">
+        <v>250</v>
+      </c>
+      <c r="D46" s="92" t="s">
         <v>251</v>
-      </c>
-      <c r="D46" s="92" t="s">
-        <v>252</v>
       </c>
       <c r="E46" s="94">
         <v>3</v>
@@ -6348,10 +6432,10 @@
         <v>180</v>
       </c>
       <c r="C47" s="93" t="s">
+        <v>252</v>
+      </c>
+      <c r="D47" s="92" t="s">
         <v>253</v>
-      </c>
-      <c r="D47" s="92" t="s">
-        <v>254</v>
       </c>
       <c r="E47" s="94">
         <v>4</v>
@@ -6367,10 +6451,10 @@
         <v>181</v>
       </c>
       <c r="C48" s="96" t="s">
+        <v>244</v>
+      </c>
+      <c r="D48" s="95" t="s">
         <v>245</v>
-      </c>
-      <c r="D48" s="95" t="s">
-        <v>246</v>
       </c>
       <c r="E48" s="97">
         <v>0</v>
@@ -6386,10 +6470,10 @@
         <v>181</v>
       </c>
       <c r="C49" s="96" t="s">
+        <v>246</v>
+      </c>
+      <c r="D49" s="95" t="s">
         <v>247</v>
-      </c>
-      <c r="D49" s="95" t="s">
-        <v>248</v>
       </c>
       <c r="E49" s="97">
         <v>1</v>
@@ -6406,10 +6490,10 @@
         <v>181</v>
       </c>
       <c r="C50" s="96" t="s">
+        <v>248</v>
+      </c>
+      <c r="D50" s="95" t="s">
         <v>249</v>
-      </c>
-      <c r="D50" s="95" t="s">
-        <v>250</v>
       </c>
       <c r="E50" s="97">
         <v>2</v>
@@ -6425,10 +6509,10 @@
         <v>181</v>
       </c>
       <c r="C51" s="96" t="s">
+        <v>250</v>
+      </c>
+      <c r="D51" s="95" t="s">
         <v>251</v>
-      </c>
-      <c r="D51" s="95" t="s">
-        <v>252</v>
       </c>
       <c r="E51" s="97">
         <v>3</v>
@@ -6444,10 +6528,10 @@
         <v>181</v>
       </c>
       <c r="C52" s="96" t="s">
+        <v>252</v>
+      </c>
+      <c r="D52" s="95" t="s">
         <v>253</v>
-      </c>
-      <c r="D52" s="95" t="s">
-        <v>254</v>
       </c>
       <c r="E52" s="97">
         <v>4</v>
@@ -6464,10 +6548,10 @@
         <v>182</v>
       </c>
       <c r="C53" s="99" t="s">
+        <v>244</v>
+      </c>
+      <c r="D53" s="98" t="s">
         <v>245</v>
-      </c>
-      <c r="D53" s="98" t="s">
-        <v>246</v>
       </c>
       <c r="E53" s="100">
         <v>0</v>
@@ -6484,10 +6568,10 @@
         <v>182</v>
       </c>
       <c r="C54" s="99" t="s">
+        <v>246</v>
+      </c>
+      <c r="D54" s="98" t="s">
         <v>247</v>
-      </c>
-      <c r="D54" s="98" t="s">
-        <v>248</v>
       </c>
       <c r="E54" s="100">
         <v>1</v>
@@ -6503,10 +6587,10 @@
         <v>182</v>
       </c>
       <c r="C55" s="99" t="s">
+        <v>248</v>
+      </c>
+      <c r="D55" s="98" t="s">
         <v>249</v>
-      </c>
-      <c r="D55" s="98" t="s">
-        <v>250</v>
       </c>
       <c r="E55" s="100">
         <v>2</v>
@@ -6522,10 +6606,10 @@
         <v>182</v>
       </c>
       <c r="C56" s="99" t="s">
+        <v>250</v>
+      </c>
+      <c r="D56" s="98" t="s">
         <v>251</v>
-      </c>
-      <c r="D56" s="98" t="s">
-        <v>252</v>
       </c>
       <c r="E56" s="100">
         <v>3</v>
@@ -6541,10 +6625,10 @@
         <v>182</v>
       </c>
       <c r="C57" s="99" t="s">
+        <v>252</v>
+      </c>
+      <c r="D57" s="98" t="s">
         <v>253</v>
-      </c>
-      <c r="D57" s="98" t="s">
-        <v>254</v>
       </c>
       <c r="E57" s="100">
         <v>4</v>
@@ -6560,10 +6644,10 @@
         <v>183</v>
       </c>
       <c r="C58" s="102" t="s">
+        <v>244</v>
+      </c>
+      <c r="D58" s="101" t="s">
         <v>245</v>
-      </c>
-      <c r="D58" s="101" t="s">
-        <v>246</v>
       </c>
       <c r="E58" s="103">
         <v>0</v>
@@ -6579,10 +6663,10 @@
         <v>183</v>
       </c>
       <c r="C59" s="102" t="s">
+        <v>246</v>
+      </c>
+      <c r="D59" s="101" t="s">
         <v>247</v>
-      </c>
-      <c r="D59" s="101" t="s">
-        <v>248</v>
       </c>
       <c r="E59" s="103">
         <v>1</v>
@@ -6599,10 +6683,10 @@
         <v>183</v>
       </c>
       <c r="C60" s="102" t="s">
+        <v>248</v>
+      </c>
+      <c r="D60" s="101" t="s">
         <v>249</v>
-      </c>
-      <c r="D60" s="101" t="s">
-        <v>250</v>
       </c>
       <c r="E60" s="103">
         <v>2</v>
@@ -6618,10 +6702,10 @@
         <v>183</v>
       </c>
       <c r="C61" s="102" t="s">
+        <v>250</v>
+      </c>
+      <c r="D61" s="101" t="s">
         <v>251</v>
-      </c>
-      <c r="D61" s="101" t="s">
-        <v>252</v>
       </c>
       <c r="E61" s="103">
         <v>3</v>
@@ -6637,10 +6721,10 @@
         <v>183</v>
       </c>
       <c r="C62" s="102" t="s">
+        <v>252</v>
+      </c>
+      <c r="D62" s="101" t="s">
         <v>253</v>
-      </c>
-      <c r="D62" s="101" t="s">
-        <v>254</v>
       </c>
       <c r="E62" s="103">
         <v>4</v>
@@ -6656,10 +6740,10 @@
         <v>184</v>
       </c>
       <c r="C63" s="105" t="s">
+        <v>244</v>
+      </c>
+      <c r="D63" s="104" t="s">
         <v>245</v>
-      </c>
-      <c r="D63" s="104" t="s">
-        <v>246</v>
       </c>
       <c r="E63" s="106">
         <v>0</v>
@@ -6675,10 +6759,10 @@
         <v>184</v>
       </c>
       <c r="C64" s="105" t="s">
+        <v>246</v>
+      </c>
+      <c r="D64" s="104" t="s">
         <v>247</v>
-      </c>
-      <c r="D64" s="104" t="s">
-        <v>248</v>
       </c>
       <c r="E64" s="106">
         <v>1</v>
@@ -6694,10 +6778,10 @@
         <v>184</v>
       </c>
       <c r="C65" s="105" t="s">
+        <v>248</v>
+      </c>
+      <c r="D65" s="104" t="s">
         <v>249</v>
-      </c>
-      <c r="D65" s="104" t="s">
-        <v>250</v>
       </c>
       <c r="E65" s="106">
         <v>2</v>
@@ -6713,10 +6797,10 @@
         <v>184</v>
       </c>
       <c r="C66" s="105" t="s">
+        <v>250</v>
+      </c>
+      <c r="D66" s="104" t="s">
         <v>251</v>
-      </c>
-      <c r="D66" s="104" t="s">
-        <v>252</v>
       </c>
       <c r="E66" s="106">
         <v>3</v>
@@ -6732,10 +6816,10 @@
         <v>184</v>
       </c>
       <c r="C67" s="105" t="s">
+        <v>252</v>
+      </c>
+      <c r="D67" s="104" t="s">
         <v>253</v>
-      </c>
-      <c r="D67" s="104" t="s">
-        <v>254</v>
       </c>
       <c r="E67" s="106">
         <v>4</v>
@@ -6751,10 +6835,10 @@
         <v>185</v>
       </c>
       <c r="C68" s="108" t="s">
+        <v>244</v>
+      </c>
+      <c r="D68" s="107" t="s">
         <v>245</v>
-      </c>
-      <c r="D68" s="107" t="s">
-        <v>246</v>
       </c>
       <c r="E68" s="109">
         <v>0</v>
@@ -6770,10 +6854,10 @@
         <v>185</v>
       </c>
       <c r="C69" s="108" t="s">
+        <v>246</v>
+      </c>
+      <c r="D69" s="107" t="s">
         <v>247</v>
-      </c>
-      <c r="D69" s="107" t="s">
-        <v>248</v>
       </c>
       <c r="E69" s="109">
         <v>1</v>
@@ -6790,10 +6874,10 @@
         <v>185</v>
       </c>
       <c r="C70" s="108" t="s">
+        <v>248</v>
+      </c>
+      <c r="D70" s="107" t="s">
         <v>249</v>
-      </c>
-      <c r="D70" s="107" t="s">
-        <v>250</v>
       </c>
       <c r="E70" s="109">
         <v>2</v>
@@ -6809,10 +6893,10 @@
         <v>185</v>
       </c>
       <c r="C71" s="108" t="s">
+        <v>250</v>
+      </c>
+      <c r="D71" s="107" t="s">
         <v>251</v>
-      </c>
-      <c r="D71" s="107" t="s">
-        <v>252</v>
       </c>
       <c r="E71" s="109">
         <v>3</v>
@@ -6828,10 +6912,10 @@
         <v>185</v>
       </c>
       <c r="C72" s="108" t="s">
+        <v>252</v>
+      </c>
+      <c r="D72" s="107" t="s">
         <v>253</v>
-      </c>
-      <c r="D72" s="107" t="s">
-        <v>254</v>
       </c>
       <c r="E72" s="109">
         <v>4</v>
@@ -6847,10 +6931,10 @@
         <v>186</v>
       </c>
       <c r="C73" s="111" t="s">
+        <v>244</v>
+      </c>
+      <c r="D73" s="110" t="s">
         <v>245</v>
-      </c>
-      <c r="D73" s="110" t="s">
-        <v>246</v>
       </c>
       <c r="E73" s="112">
         <v>0</v>
@@ -6866,10 +6950,10 @@
         <v>186</v>
       </c>
       <c r="C74" s="111" t="s">
+        <v>246</v>
+      </c>
+      <c r="D74" s="110" t="s">
         <v>247</v>
-      </c>
-      <c r="D74" s="110" t="s">
-        <v>248</v>
       </c>
       <c r="E74" s="112">
         <v>1</v>
@@ -6885,10 +6969,10 @@
         <v>186</v>
       </c>
       <c r="C75" s="111" t="s">
+        <v>248</v>
+      </c>
+      <c r="D75" s="110" t="s">
         <v>249</v>
-      </c>
-      <c r="D75" s="110" t="s">
-        <v>250</v>
       </c>
       <c r="E75" s="112">
         <v>2</v>
@@ -6904,10 +6988,10 @@
         <v>186</v>
       </c>
       <c r="C76" s="111" t="s">
+        <v>250</v>
+      </c>
+      <c r="D76" s="110" t="s">
         <v>251</v>
-      </c>
-      <c r="D76" s="110" t="s">
-        <v>252</v>
       </c>
       <c r="E76" s="112">
         <v>3</v>
@@ -6923,10 +7007,10 @@
         <v>186</v>
       </c>
       <c r="C77" s="111" t="s">
+        <v>252</v>
+      </c>
+      <c r="D77" s="110" t="s">
         <v>253</v>
-      </c>
-      <c r="D77" s="110" t="s">
-        <v>254</v>
       </c>
       <c r="E77" s="112">
         <v>4</v>
@@ -6943,10 +7027,10 @@
         <v>187</v>
       </c>
       <c r="C78" s="114" t="s">
+        <v>244</v>
+      </c>
+      <c r="D78" s="113" t="s">
         <v>245</v>
-      </c>
-      <c r="D78" s="113" t="s">
-        <v>246</v>
       </c>
       <c r="E78" s="115">
         <v>0</v>
@@ -6962,10 +7046,10 @@
         <v>187</v>
       </c>
       <c r="C79" s="114" t="s">
+        <v>246</v>
+      </c>
+      <c r="D79" s="113" t="s">
         <v>247</v>
-      </c>
-      <c r="D79" s="113" t="s">
-        <v>248</v>
       </c>
       <c r="E79" s="115">
         <v>1</v>
@@ -6981,10 +7065,10 @@
         <v>187</v>
       </c>
       <c r="C80" s="114" t="s">
+        <v>248</v>
+      </c>
+      <c r="D80" s="113" t="s">
         <v>249</v>
-      </c>
-      <c r="D80" s="113" t="s">
-        <v>250</v>
       </c>
       <c r="E80" s="115">
         <v>2</v>
@@ -7000,10 +7084,10 @@
         <v>187</v>
       </c>
       <c r="C81" s="114" t="s">
+        <v>250</v>
+      </c>
+      <c r="D81" s="113" t="s">
         <v>251</v>
-      </c>
-      <c r="D81" s="113" t="s">
-        <v>252</v>
       </c>
       <c r="E81" s="115">
         <v>3</v>
@@ -7019,10 +7103,10 @@
         <v>187</v>
       </c>
       <c r="C82" s="114" t="s">
+        <v>252</v>
+      </c>
+      <c r="D82" s="113" t="s">
         <v>253</v>
-      </c>
-      <c r="D82" s="113" t="s">
-        <v>254</v>
       </c>
       <c r="E82" s="115">
         <v>4</v>
@@ -7038,10 +7122,10 @@
         <v>188</v>
       </c>
       <c r="C83" s="117" t="s">
+        <v>244</v>
+      </c>
+      <c r="D83" s="116" t="s">
         <v>245</v>
-      </c>
-      <c r="D83" s="116" t="s">
-        <v>246</v>
       </c>
       <c r="E83" s="118">
         <v>0</v>
@@ -7057,10 +7141,10 @@
         <v>188</v>
       </c>
       <c r="C84" s="117" t="s">
+        <v>246</v>
+      </c>
+      <c r="D84" s="116" t="s">
         <v>247</v>
-      </c>
-      <c r="D84" s="116" t="s">
-        <v>248</v>
       </c>
       <c r="E84" s="118">
         <v>1</v>
@@ -7076,10 +7160,10 @@
         <v>188</v>
       </c>
       <c r="C85" s="117" t="s">
+        <v>248</v>
+      </c>
+      <c r="D85" s="116" t="s">
         <v>249</v>
-      </c>
-      <c r="D85" s="116" t="s">
-        <v>250</v>
       </c>
       <c r="E85" s="118">
         <v>2</v>
@@ -7095,10 +7179,10 @@
         <v>188</v>
       </c>
       <c r="C86" s="117" t="s">
+        <v>250</v>
+      </c>
+      <c r="D86" s="116" t="s">
         <v>251</v>
-      </c>
-      <c r="D86" s="116" t="s">
-        <v>252</v>
       </c>
       <c r="E86" s="118">
         <v>3</v>
@@ -7114,10 +7198,10 @@
         <v>188</v>
       </c>
       <c r="C87" s="117" t="s">
+        <v>252</v>
+      </c>
+      <c r="D87" s="116" t="s">
         <v>253</v>
-      </c>
-      <c r="D87" s="116" t="s">
-        <v>254</v>
       </c>
       <c r="E87" s="118">
         <v>4</v>
@@ -7133,10 +7217,10 @@
         <v>189</v>
       </c>
       <c r="C88" s="120" t="s">
+        <v>244</v>
+      </c>
+      <c r="D88" s="119" t="s">
         <v>245</v>
-      </c>
-      <c r="D88" s="119" t="s">
-        <v>246</v>
       </c>
       <c r="E88" s="121">
         <v>0</v>
@@ -7152,10 +7236,10 @@
         <v>189</v>
       </c>
       <c r="C89" s="120" t="s">
+        <v>246</v>
+      </c>
+      <c r="D89" s="119" t="s">
         <v>247</v>
-      </c>
-      <c r="D89" s="119" t="s">
-        <v>248</v>
       </c>
       <c r="E89" s="121">
         <v>1</v>
@@ -7171,10 +7255,10 @@
         <v>189</v>
       </c>
       <c r="C90" s="120" t="s">
+        <v>248</v>
+      </c>
+      <c r="D90" s="119" t="s">
         <v>249</v>
-      </c>
-      <c r="D90" s="119" t="s">
-        <v>250</v>
       </c>
       <c r="E90" s="121">
         <v>2</v>
@@ -7190,10 +7274,10 @@
         <v>189</v>
       </c>
       <c r="C91" s="120" t="s">
+        <v>250</v>
+      </c>
+      <c r="D91" s="119" t="s">
         <v>251</v>
-      </c>
-      <c r="D91" s="119" t="s">
-        <v>252</v>
       </c>
       <c r="E91" s="121">
         <v>3</v>
@@ -7209,10 +7293,10 @@
         <v>189</v>
       </c>
       <c r="C92" s="120" t="s">
+        <v>252</v>
+      </c>
+      <c r="D92" s="119" t="s">
         <v>253</v>
-      </c>
-      <c r="D92" s="119" t="s">
-        <v>254</v>
       </c>
       <c r="E92" s="121">
         <v>4</v>
@@ -7228,10 +7312,10 @@
         <v>190</v>
       </c>
       <c r="C93" s="123" t="s">
+        <v>244</v>
+      </c>
+      <c r="D93" s="122" t="s">
         <v>245</v>
-      </c>
-      <c r="D93" s="122" t="s">
-        <v>246</v>
       </c>
       <c r="E93" s="124">
         <v>0</v>
@@ -7247,10 +7331,10 @@
         <v>190</v>
       </c>
       <c r="C94" s="123" t="s">
+        <v>246</v>
+      </c>
+      <c r="D94" s="122" t="s">
         <v>247</v>
-      </c>
-      <c r="D94" s="122" t="s">
-        <v>248</v>
       </c>
       <c r="E94" s="124">
         <v>1</v>
@@ -7267,10 +7351,10 @@
         <v>190</v>
       </c>
       <c r="C95" s="123" t="s">
+        <v>248</v>
+      </c>
+      <c r="D95" s="122" t="s">
         <v>249</v>
-      </c>
-      <c r="D95" s="122" t="s">
-        <v>250</v>
       </c>
       <c r="E95" s="124">
         <v>2</v>
@@ -7286,10 +7370,10 @@
         <v>190</v>
       </c>
       <c r="C96" s="123" t="s">
+        <v>250</v>
+      </c>
+      <c r="D96" s="122" t="s">
         <v>251</v>
-      </c>
-      <c r="D96" s="122" t="s">
-        <v>252</v>
       </c>
       <c r="E96" s="124">
         <v>3</v>
@@ -7305,10 +7389,10 @@
         <v>190</v>
       </c>
       <c r="C97" s="123" t="s">
+        <v>252</v>
+      </c>
+      <c r="D97" s="122" t="s">
         <v>253</v>
-      </c>
-      <c r="D97" s="122" t="s">
-        <v>254</v>
       </c>
       <c r="E97" s="124">
         <v>4</v>
@@ -7324,10 +7408,10 @@
         <v>191</v>
       </c>
       <c r="C98" s="126" t="s">
+        <v>244</v>
+      </c>
+      <c r="D98" s="125" t="s">
         <v>245</v>
-      </c>
-      <c r="D98" s="125" t="s">
-        <v>246</v>
       </c>
       <c r="E98" s="127">
         <v>0</v>
@@ -7343,10 +7427,10 @@
         <v>191</v>
       </c>
       <c r="C99" s="126" t="s">
+        <v>246</v>
+      </c>
+      <c r="D99" s="125" t="s">
         <v>247</v>
-      </c>
-      <c r="D99" s="125" t="s">
-        <v>248</v>
       </c>
       <c r="E99" s="127">
         <v>1</v>
@@ -7362,10 +7446,10 @@
         <v>191</v>
       </c>
       <c r="C100" s="126" t="s">
+        <v>248</v>
+      </c>
+      <c r="D100" s="125" t="s">
         <v>249</v>
-      </c>
-      <c r="D100" s="125" t="s">
-        <v>250</v>
       </c>
       <c r="E100" s="127">
         <v>2</v>
@@ -7381,10 +7465,10 @@
         <v>191</v>
       </c>
       <c r="C101" s="126" t="s">
+        <v>250</v>
+      </c>
+      <c r="D101" s="125" t="s">
         <v>251</v>
-      </c>
-      <c r="D101" s="125" t="s">
-        <v>252</v>
       </c>
       <c r="E101" s="127">
         <v>3</v>
@@ -7400,10 +7484,10 @@
         <v>191</v>
       </c>
       <c r="C102" s="126" t="s">
+        <v>252</v>
+      </c>
+      <c r="D102" s="125" t="s">
         <v>253</v>
-      </c>
-      <c r="D102" s="125" t="s">
-        <v>254</v>
       </c>
       <c r="E102" s="127">
         <v>4</v>
@@ -7420,10 +7504,10 @@
         <v>192</v>
       </c>
       <c r="C103" s="129" t="s">
+        <v>244</v>
+      </c>
+      <c r="D103" s="128" t="s">
         <v>245</v>
-      </c>
-      <c r="D103" s="128" t="s">
-        <v>246</v>
       </c>
       <c r="E103" s="130">
         <v>0</v>
@@ -7439,10 +7523,10 @@
         <v>192</v>
       </c>
       <c r="C104" s="129" t="s">
+        <v>246</v>
+      </c>
+      <c r="D104" s="128" t="s">
         <v>247</v>
-      </c>
-      <c r="D104" s="128" t="s">
-        <v>248</v>
       </c>
       <c r="E104" s="130">
         <v>1</v>
@@ -7458,10 +7542,10 @@
         <v>192</v>
       </c>
       <c r="C105" s="129" t="s">
+        <v>248</v>
+      </c>
+      <c r="D105" s="128" t="s">
         <v>249</v>
-      </c>
-      <c r="D105" s="128" t="s">
-        <v>250</v>
       </c>
       <c r="E105" s="130">
         <v>2</v>
@@ -7477,10 +7561,10 @@
         <v>192</v>
       </c>
       <c r="C106" s="129" t="s">
+        <v>250</v>
+      </c>
+      <c r="D106" s="128" t="s">
         <v>251</v>
-      </c>
-      <c r="D106" s="128" t="s">
-        <v>252</v>
       </c>
       <c r="E106" s="130">
         <v>3</v>
@@ -7496,10 +7580,10 @@
         <v>192</v>
       </c>
       <c r="C107" s="129" t="s">
+        <v>252</v>
+      </c>
+      <c r="D107" s="128" t="s">
         <v>253</v>
-      </c>
-      <c r="D107" s="128" t="s">
-        <v>254</v>
       </c>
       <c r="E107" s="130">
         <v>4</v>
@@ -7515,10 +7599,10 @@
         <v>193</v>
       </c>
       <c r="C108" s="132" t="s">
+        <v>244</v>
+      </c>
+      <c r="D108" s="131" t="s">
         <v>245</v>
-      </c>
-      <c r="D108" s="131" t="s">
-        <v>246</v>
       </c>
       <c r="E108" s="133">
         <v>0</v>
@@ -7535,10 +7619,10 @@
         <v>193</v>
       </c>
       <c r="C109" s="132" t="s">
+        <v>246</v>
+      </c>
+      <c r="D109" s="131" t="s">
         <v>247</v>
-      </c>
-      <c r="D109" s="131" t="s">
-        <v>248</v>
       </c>
       <c r="E109" s="133">
         <v>1</v>
@@ -7556,10 +7640,10 @@
         <v>193</v>
       </c>
       <c r="C110" s="132" t="s">
+        <v>248</v>
+      </c>
+      <c r="D110" s="131" t="s">
         <v>249</v>
-      </c>
-      <c r="D110" s="131" t="s">
-        <v>250</v>
       </c>
       <c r="E110" s="133">
         <v>2</v>
@@ -7576,10 +7660,10 @@
         <v>193</v>
       </c>
       <c r="C111" s="132" t="s">
+        <v>250</v>
+      </c>
+      <c r="D111" s="131" t="s">
         <v>251</v>
-      </c>
-      <c r="D111" s="131" t="s">
-        <v>252</v>
       </c>
       <c r="E111" s="133">
         <v>3</v>
@@ -7595,10 +7679,10 @@
         <v>193</v>
       </c>
       <c r="C112" s="132" t="s">
+        <v>252</v>
+      </c>
+      <c r="D112" s="131" t="s">
         <v>253</v>
-      </c>
-      <c r="D112" s="131" t="s">
-        <v>254</v>
       </c>
       <c r="E112" s="133">
         <v>4</v>
@@ -7614,10 +7698,10 @@
         <v>194</v>
       </c>
       <c r="C113" s="135" t="s">
+        <v>244</v>
+      </c>
+      <c r="D113" s="134" t="s">
         <v>245</v>
-      </c>
-      <c r="D113" s="134" t="s">
-        <v>246</v>
       </c>
       <c r="E113" s="136">
         <v>0</v>
@@ -7633,10 +7717,10 @@
         <v>194</v>
       </c>
       <c r="C114" s="135" t="s">
+        <v>246</v>
+      </c>
+      <c r="D114" s="134" t="s">
         <v>247</v>
-      </c>
-      <c r="D114" s="134" t="s">
-        <v>248</v>
       </c>
       <c r="E114" s="136">
         <v>1</v>
@@ -7652,10 +7736,10 @@
         <v>194</v>
       </c>
       <c r="C115" s="135" t="s">
+        <v>248</v>
+      </c>
+      <c r="D115" s="134" t="s">
         <v>249</v>
-      </c>
-      <c r="D115" s="134" t="s">
-        <v>250</v>
       </c>
       <c r="E115" s="136">
         <v>2</v>
@@ -7671,10 +7755,10 @@
         <v>194</v>
       </c>
       <c r="C116" s="135" t="s">
+        <v>250</v>
+      </c>
+      <c r="D116" s="134" t="s">
         <v>251</v>
-      </c>
-      <c r="D116" s="134" t="s">
-        <v>252</v>
       </c>
       <c r="E116" s="136">
         <v>3</v>
@@ -7690,10 +7774,10 @@
         <v>194</v>
       </c>
       <c r="C117" s="135" t="s">
+        <v>252</v>
+      </c>
+      <c r="D117" s="134" t="s">
         <v>253</v>
-      </c>
-      <c r="D117" s="134" t="s">
-        <v>254</v>
       </c>
       <c r="E117" s="136">
         <v>4</v>
@@ -7709,10 +7793,10 @@
         <v>195</v>
       </c>
       <c r="C118" s="138" t="s">
+        <v>244</v>
+      </c>
+      <c r="D118" s="137" t="s">
         <v>245</v>
-      </c>
-      <c r="D118" s="137" t="s">
-        <v>246</v>
       </c>
       <c r="E118" s="139">
         <v>0</v>
@@ -7728,10 +7812,10 @@
         <v>195</v>
       </c>
       <c r="C119" s="138" t="s">
+        <v>246</v>
+      </c>
+      <c r="D119" s="137" t="s">
         <v>247</v>
-      </c>
-      <c r="D119" s="137" t="s">
-        <v>248</v>
       </c>
       <c r="E119" s="139">
         <v>1</v>
@@ -7747,10 +7831,10 @@
         <v>195</v>
       </c>
       <c r="C120" s="138" t="s">
+        <v>248</v>
+      </c>
+      <c r="D120" s="137" t="s">
         <v>249</v>
-      </c>
-      <c r="D120" s="137" t="s">
-        <v>250</v>
       </c>
       <c r="E120" s="139">
         <v>2</v>
@@ -7766,10 +7850,10 @@
         <v>195</v>
       </c>
       <c r="C121" s="138" t="s">
+        <v>250</v>
+      </c>
+      <c r="D121" s="137" t="s">
         <v>251</v>
-      </c>
-      <c r="D121" s="137" t="s">
-        <v>252</v>
       </c>
       <c r="E121" s="139">
         <v>3</v>
@@ -7785,10 +7869,10 @@
         <v>195</v>
       </c>
       <c r="C122" s="138" t="s">
+        <v>252</v>
+      </c>
+      <c r="D122" s="137" t="s">
         <v>253</v>
-      </c>
-      <c r="D122" s="137" t="s">
-        <v>254</v>
       </c>
       <c r="E122" s="139">
         <v>4</v>
@@ -7805,10 +7889,10 @@
         <v>196</v>
       </c>
       <c r="C123" s="141" t="s">
+        <v>244</v>
+      </c>
+      <c r="D123" s="140" t="s">
         <v>245</v>
-      </c>
-      <c r="D123" s="140" t="s">
-        <v>246</v>
       </c>
       <c r="E123" s="142">
         <v>0</v>
@@ -7825,10 +7909,10 @@
         <v>196</v>
       </c>
       <c r="C124" s="141" t="s">
+        <v>246</v>
+      </c>
+      <c r="D124" s="140" t="s">
         <v>247</v>
-      </c>
-      <c r="D124" s="140" t="s">
-        <v>248</v>
       </c>
       <c r="E124" s="142">
         <v>1</v>
@@ -7844,10 +7928,10 @@
         <v>196</v>
       </c>
       <c r="C125" s="141" t="s">
+        <v>248</v>
+      </c>
+      <c r="D125" s="140" t="s">
         <v>249</v>
-      </c>
-      <c r="D125" s="140" t="s">
-        <v>250</v>
       </c>
       <c r="E125" s="142">
         <v>2</v>
@@ -7863,10 +7947,10 @@
         <v>196</v>
       </c>
       <c r="C126" s="141" t="s">
+        <v>250</v>
+      </c>
+      <c r="D126" s="140" t="s">
         <v>251</v>
-      </c>
-      <c r="D126" s="140" t="s">
-        <v>252</v>
       </c>
       <c r="E126" s="142">
         <v>3</v>
@@ -7882,10 +7966,10 @@
         <v>196</v>
       </c>
       <c r="C127" s="141" t="s">
+        <v>252</v>
+      </c>
+      <c r="D127" s="140" t="s">
         <v>253</v>
-      </c>
-      <c r="D127" s="140" t="s">
-        <v>254</v>
       </c>
       <c r="E127" s="142">
         <v>4</v>
@@ -7902,10 +7986,10 @@
         <v>197</v>
       </c>
       <c r="C128" s="144" t="s">
+        <v>244</v>
+      </c>
+      <c r="D128" s="143" t="s">
         <v>245</v>
-      </c>
-      <c r="D128" s="143" t="s">
-        <v>246</v>
       </c>
       <c r="E128" s="145">
         <v>0</v>
@@ -7921,10 +8005,10 @@
         <v>197</v>
       </c>
       <c r="C129" s="144" t="s">
+        <v>246</v>
+      </c>
+      <c r="D129" s="143" t="s">
         <v>247</v>
-      </c>
-      <c r="D129" s="143" t="s">
-        <v>248</v>
       </c>
       <c r="E129" s="145">
         <v>1</v>
@@ -7940,10 +8024,10 @@
         <v>197</v>
       </c>
       <c r="C130" s="144" t="s">
+        <v>248</v>
+      </c>
+      <c r="D130" s="143" t="s">
         <v>249</v>
-      </c>
-      <c r="D130" s="143" t="s">
-        <v>250</v>
       </c>
       <c r="E130" s="145">
         <v>2</v>
@@ -7959,10 +8043,10 @@
         <v>197</v>
       </c>
       <c r="C131" s="144" t="s">
+        <v>250</v>
+      </c>
+      <c r="D131" s="143" t="s">
         <v>251</v>
-      </c>
-      <c r="D131" s="143" t="s">
-        <v>252</v>
       </c>
       <c r="E131" s="145">
         <v>3</v>
@@ -7978,10 +8062,10 @@
         <v>197</v>
       </c>
       <c r="C132" s="144" t="s">
+        <v>252</v>
+      </c>
+      <c r="D132" s="143" t="s">
         <v>253</v>
-      </c>
-      <c r="D132" s="143" t="s">
-        <v>254</v>
       </c>
       <c r="E132" s="145">
         <v>4</v>
@@ -7997,10 +8081,10 @@
         <v>198</v>
       </c>
       <c r="C133" s="147" t="s">
+        <v>244</v>
+      </c>
+      <c r="D133" s="146" t="s">
         <v>245</v>
-      </c>
-      <c r="D133" s="146" t="s">
-        <v>246</v>
       </c>
       <c r="E133" s="148">
         <v>0</v>
@@ -8016,10 +8100,10 @@
         <v>198</v>
       </c>
       <c r="C134" s="147" t="s">
+        <v>246</v>
+      </c>
+      <c r="D134" s="146" t="s">
         <v>247</v>
-      </c>
-      <c r="D134" s="146" t="s">
-        <v>248</v>
       </c>
       <c r="E134" s="148">
         <v>1</v>
@@ -8035,10 +8119,10 @@
         <v>198</v>
       </c>
       <c r="C135" s="147" t="s">
+        <v>248</v>
+      </c>
+      <c r="D135" s="146" t="s">
         <v>249</v>
-      </c>
-      <c r="D135" s="146" t="s">
-        <v>250</v>
       </c>
       <c r="E135" s="148">
         <v>2</v>
@@ -8054,10 +8138,10 @@
         <v>198</v>
       </c>
       <c r="C136" s="147" t="s">
+        <v>250</v>
+      </c>
+      <c r="D136" s="146" t="s">
         <v>251</v>
-      </c>
-      <c r="D136" s="146" t="s">
-        <v>252</v>
       </c>
       <c r="E136" s="148">
         <v>3</v>
@@ -8073,10 +8157,10 @@
         <v>198</v>
       </c>
       <c r="C137" s="147" t="s">
+        <v>252</v>
+      </c>
+      <c r="D137" s="146" t="s">
         <v>253</v>
-      </c>
-      <c r="D137" s="146" t="s">
-        <v>254</v>
       </c>
       <c r="E137" s="148">
         <v>4</v>
@@ -8093,10 +8177,10 @@
         <v>199</v>
       </c>
       <c r="C138" s="150" t="s">
+        <v>244</v>
+      </c>
+      <c r="D138" s="149" t="s">
         <v>245</v>
-      </c>
-      <c r="D138" s="149" t="s">
-        <v>246</v>
       </c>
       <c r="E138" s="151">
         <v>0</v>
@@ -8113,10 +8197,10 @@
         <v>199</v>
       </c>
       <c r="C139" s="150" t="s">
+        <v>246</v>
+      </c>
+      <c r="D139" s="149" t="s">
         <v>247</v>
-      </c>
-      <c r="D139" s="149" t="s">
-        <v>248</v>
       </c>
       <c r="E139" s="151">
         <v>1</v>
@@ -8132,10 +8216,10 @@
         <v>199</v>
       </c>
       <c r="C140" s="150" t="s">
+        <v>248</v>
+      </c>
+      <c r="D140" s="149" t="s">
         <v>249</v>
-      </c>
-      <c r="D140" s="149" t="s">
-        <v>250</v>
       </c>
       <c r="E140" s="151">
         <v>2</v>
@@ -8151,10 +8235,10 @@
         <v>199</v>
       </c>
       <c r="C141" s="150" t="s">
+        <v>250</v>
+      </c>
+      <c r="D141" s="149" t="s">
         <v>251</v>
-      </c>
-      <c r="D141" s="149" t="s">
-        <v>252</v>
       </c>
       <c r="E141" s="151">
         <v>3</v>
@@ -8170,10 +8254,10 @@
         <v>199</v>
       </c>
       <c r="C142" s="150" t="s">
+        <v>252</v>
+      </c>
+      <c r="D142" s="149" t="s">
         <v>253</v>
-      </c>
-      <c r="D142" s="149" t="s">
-        <v>254</v>
       </c>
       <c r="E142" s="151">
         <v>4</v>
@@ -8189,10 +8273,10 @@
         <v>200</v>
       </c>
       <c r="C143" s="153" t="s">
+        <v>244</v>
+      </c>
+      <c r="D143" s="152" t="s">
         <v>245</v>
-      </c>
-      <c r="D143" s="152" t="s">
-        <v>246</v>
       </c>
       <c r="E143" s="154">
         <v>0</v>
@@ -8208,10 +8292,10 @@
         <v>200</v>
       </c>
       <c r="C144" s="153" t="s">
+        <v>246</v>
+      </c>
+      <c r="D144" s="152" t="s">
         <v>247</v>
-      </c>
-      <c r="D144" s="152" t="s">
-        <v>248</v>
       </c>
       <c r="E144" s="154">
         <v>1</v>
@@ -8227,10 +8311,10 @@
         <v>200</v>
       </c>
       <c r="C145" s="153" t="s">
+        <v>248</v>
+      </c>
+      <c r="D145" s="152" t="s">
         <v>249</v>
-      </c>
-      <c r="D145" s="152" t="s">
-        <v>250</v>
       </c>
       <c r="E145" s="154">
         <v>2</v>
@@ -8246,10 +8330,10 @@
         <v>200</v>
       </c>
       <c r="C146" s="153" t="s">
+        <v>250</v>
+      </c>
+      <c r="D146" s="152" t="s">
         <v>251</v>
-      </c>
-      <c r="D146" s="152" t="s">
-        <v>252</v>
       </c>
       <c r="E146" s="154">
         <v>3</v>
@@ -8265,10 +8349,10 @@
         <v>200</v>
       </c>
       <c r="C147" s="153" t="s">
+        <v>252</v>
+      </c>
+      <c r="D147" s="152" t="s">
         <v>253</v>
-      </c>
-      <c r="D147" s="152" t="s">
-        <v>254</v>
       </c>
       <c r="E147" s="154">
         <v>4</v>
@@ -8284,10 +8368,10 @@
         <v>201</v>
       </c>
       <c r="C148" s="156" t="s">
+        <v>244</v>
+      </c>
+      <c r="D148" s="155" t="s">
         <v>245</v>
-      </c>
-      <c r="D148" s="155" t="s">
-        <v>246</v>
       </c>
       <c r="E148" s="157">
         <v>0</v>
@@ -8303,10 +8387,10 @@
         <v>201</v>
       </c>
       <c r="C149" s="156" t="s">
+        <v>246</v>
+      </c>
+      <c r="D149" s="155" t="s">
         <v>247</v>
-      </c>
-      <c r="D149" s="155" t="s">
-        <v>248</v>
       </c>
       <c r="E149" s="157">
         <v>1</v>
@@ -8322,10 +8406,10 @@
         <v>201</v>
       </c>
       <c r="C150" s="156" t="s">
+        <v>248</v>
+      </c>
+      <c r="D150" s="155" t="s">
         <v>249</v>
-      </c>
-      <c r="D150" s="155" t="s">
-        <v>250</v>
       </c>
       <c r="E150" s="157">
         <v>2</v>
@@ -8341,10 +8425,10 @@
         <v>201</v>
       </c>
       <c r="C151" s="156" t="s">
+        <v>250</v>
+      </c>
+      <c r="D151" s="155" t="s">
         <v>251</v>
-      </c>
-      <c r="D151" s="155" t="s">
-        <v>252</v>
       </c>
       <c r="E151" s="157">
         <v>3</v>
@@ -8360,10 +8444,10 @@
         <v>201</v>
       </c>
       <c r="C152" s="156" t="s">
+        <v>252</v>
+      </c>
+      <c r="D152" s="155" t="s">
         <v>253</v>
-      </c>
-      <c r="D152" s="155" t="s">
-        <v>254</v>
       </c>
       <c r="E152" s="157">
         <v>4</v>
@@ -8379,10 +8463,10 @@
         <v>202</v>
       </c>
       <c r="C153" s="159" t="s">
+        <v>244</v>
+      </c>
+      <c r="D153" s="158" t="s">
         <v>245</v>
-      </c>
-      <c r="D153" s="158" t="s">
-        <v>246</v>
       </c>
       <c r="E153" s="160">
         <v>0</v>
@@ -8398,10 +8482,10 @@
         <v>202</v>
       </c>
       <c r="C154" s="159" t="s">
+        <v>246</v>
+      </c>
+      <c r="D154" s="158" t="s">
         <v>247</v>
-      </c>
-      <c r="D154" s="158" t="s">
-        <v>248</v>
       </c>
       <c r="E154" s="160">
         <v>1</v>
@@ -8418,10 +8502,10 @@
         <v>202</v>
       </c>
       <c r="C155" s="159" t="s">
+        <v>248</v>
+      </c>
+      <c r="D155" s="158" t="s">
         <v>249</v>
-      </c>
-      <c r="D155" s="158" t="s">
-        <v>250</v>
       </c>
       <c r="E155" s="160">
         <v>2</v>
@@ -8437,10 +8521,10 @@
         <v>202</v>
       </c>
       <c r="C156" s="159" t="s">
+        <v>250</v>
+      </c>
+      <c r="D156" s="158" t="s">
         <v>251</v>
-      </c>
-      <c r="D156" s="158" t="s">
-        <v>252</v>
       </c>
       <c r="E156" s="160">
         <v>3</v>
@@ -8456,10 +8540,10 @@
         <v>202</v>
       </c>
       <c r="C157" s="159" t="s">
+        <v>252</v>
+      </c>
+      <c r="D157" s="158" t="s">
         <v>253</v>
-      </c>
-      <c r="D157" s="158" t="s">
-        <v>254</v>
       </c>
       <c r="E157" s="160">
         <v>4</v>
@@ -8475,10 +8559,10 @@
         <v>203</v>
       </c>
       <c r="C158" s="163" t="s">
+        <v>244</v>
+      </c>
+      <c r="D158" s="162" t="s">
         <v>245</v>
-      </c>
-      <c r="D158" s="162" t="s">
-        <v>246</v>
       </c>
       <c r="E158" s="164">
         <v>0</v>
@@ -8494,10 +8578,10 @@
         <v>203</v>
       </c>
       <c r="C159" s="163" t="s">
+        <v>246</v>
+      </c>
+      <c r="D159" s="162" t="s">
         <v>247</v>
-      </c>
-      <c r="D159" s="162" t="s">
-        <v>248</v>
       </c>
       <c r="E159" s="164">
         <v>1</v>
@@ -8513,10 +8597,10 @@
         <v>203</v>
       </c>
       <c r="C160" s="163" t="s">
+        <v>248</v>
+      </c>
+      <c r="D160" s="162" t="s">
         <v>249</v>
-      </c>
-      <c r="D160" s="162" t="s">
-        <v>250</v>
       </c>
       <c r="E160" s="164">
         <v>2</v>
@@ -8532,10 +8616,10 @@
         <v>203</v>
       </c>
       <c r="C161" s="163" t="s">
+        <v>250</v>
+      </c>
+      <c r="D161" s="162" t="s">
         <v>251</v>
-      </c>
-      <c r="D161" s="162" t="s">
-        <v>252</v>
       </c>
       <c r="E161" s="164">
         <v>3</v>
@@ -8551,10 +8635,10 @@
         <v>203</v>
       </c>
       <c r="C162" s="163" t="s">
+        <v>252</v>
+      </c>
+      <c r="D162" s="162" t="s">
         <v>253</v>
-      </c>
-      <c r="D162" s="162" t="s">
-        <v>254</v>
       </c>
       <c r="E162" s="164">
         <v>4</v>

</xml_diff>